<commit_message>
diagrama, guia de arquitetura, e gantt
</commit_message>
<xml_diff>
--- a/Documentação/Arquitetura/Guia Definicao da Arquitetura V4.xlsx
+++ b/Documentação/Arquitetura/Guia Definicao da Arquitetura V4.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
   <si>
     <t xml:space="preserve">ANÁLISE</t>
   </si>
@@ -49,7 +49,7 @@
     <t xml:space="preserve">Interfaces de integração </t>
   </si>
   <si>
-    <t xml:space="preserve">Exemplo: Web Service RESTAPI</t>
+    <t xml:space="preserve">Api Picpay</t>
   </si>
   <si>
     <t xml:space="preserve">Camada de acesso aos dados</t>
@@ -94,16 +94,7 @@
     <t xml:space="preserve">Configuração da IDE de deploy automatizado</t>
   </si>
   <si>
-    <t xml:space="preserve">Exemplo: Azure DevOps</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Segurança </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Definição do modelo de autenticação </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Exemplo: Token ou SSO Com Google</t>
+    <t xml:space="preserve">Vercel</t>
   </si>
   <si>
     <t xml:space="preserve">INFRA</t>
@@ -133,7 +124,7 @@
     <t xml:space="preserve">Servidor de Aplicações, SDKs, Bibliotecas</t>
   </si>
   <si>
-    <t xml:space="preserve">Jdk, </t>
+    <t xml:space="preserve">JDK, leaflet, viacep ,styled-components </t>
   </si>
   <si>
     <t xml:space="preserve">Hardware/Provisionamento Cloud</t>
@@ -181,7 +172,7 @@
     <t xml:space="preserve">Ferramenta para gestão do projeto, rastreabilidade, gestão de mudanças.</t>
   </si>
   <si>
-    <t xml:space="preserve">Trello inicialmente migramos para o Jira</t>
+    <t xml:space="preserve">Trello, Jira</t>
   </si>
   <si>
     <t xml:space="preserve">Edição</t>
@@ -209,12 +200,6 @@
   </si>
   <si>
     <t xml:space="preserve">Definido que deve ser o GITHUB da Faculdade, criar release Notes de Versão.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Testes </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Processo e ferramenta para realização dos Testes</t>
   </si>
 </sst>
 </file>
@@ -297,7 +282,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="13">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -345,6 +330,48 @@
       <right style="thin"/>
       <top/>
       <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right/>
+      <top style="hair"/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top style="hair"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="hair"/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="hair"/>
+      <top/>
+      <bottom style="hair"/>
       <diagonal/>
     </border>
   </borders>
@@ -373,7 +400,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -422,43 +449,51 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="1"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="1"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="1"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="1"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="1"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="1"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="1"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="1"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false" readingOrder="1"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -486,7 +521,7 @@
   <dimension ref="A1:D1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
+      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="56.015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -596,45 +631,45 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="6"/>
-      <c r="B9" s="12" t="s">
+    <row r="10" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="B10" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="C10" s="7" t="s">
         <v>27</v>
       </c>
+      <c r="D10" s="12" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="B11" s="7" t="s">
+      <c r="A11" s="6"/>
+      <c r="B11" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="D11" s="14" t="s">
+      <c r="D11" s="11" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="6"/>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C12" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D12" s="11" t="s">
+      <c r="D12" s="13" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="6"/>
       <c r="B13" s="2" t="s">
         <v>35</v>
@@ -642,128 +677,108 @@
       <c r="C13" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D13" s="15" t="s">
+      <c r="D13" s="13" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="6"/>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="D14" s="15" t="s">
+      <c r="D14" s="16" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="6"/>
-      <c r="B15" s="16" t="s">
+    <row r="16" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="C15" s="17" t="s">
+      <c r="B16" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="D15" s="13" t="s">
+      <c r="C16" s="19" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="17" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="6" t="s">
+      <c r="D16" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="B17" s="18" t="s">
+    </row>
+    <row r="17" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="17"/>
+      <c r="B17" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C17" s="19" t="s">
+      <c r="C17" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="D17" s="20" t="s">
+      <c r="D17" s="21" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="47.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="6"/>
+    <row r="18" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="17"/>
       <c r="B18" s="2" t="s">
         <v>48</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D18" s="15" t="s">
+      <c r="D18" s="21" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="6"/>
+    <row r="19" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="17"/>
       <c r="B19" s="2" t="s">
         <v>51</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="D19" s="15" t="s">
+      <c r="D19" s="21" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="6"/>
+    <row r="20" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="17"/>
       <c r="B20" s="2" t="s">
         <v>54</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D20" s="15" t="s">
+      <c r="D20" s="21" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="6"/>
-      <c r="B21" s="2" t="s">
+    <row r="21" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="17"/>
+      <c r="B21" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C21" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="D21" s="15" t="s">
+      <c r="D21" s="23" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="6"/>
-      <c r="B22" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="C22" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="D22" s="10" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="6"/>
-      <c r="B23" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="C23" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="D23" s="21"/>
-    </row>
-    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="22"/>
-    </row>
+    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="24"/>
+    </row>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A2:A9"/>
-    <mergeCell ref="A11:A15"/>
-    <mergeCell ref="A17:A23"/>
+    <mergeCell ref="A2:A8"/>
+    <mergeCell ref="A10:A14"/>
+    <mergeCell ref="A16:A21"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.511805555555555" right="0.511805555555555" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>